<commit_message>
update 1 số thứ lên
</commit_message>
<xml_diff>
--- a/5_TuningPrompting/output_data_v2.xlsx
+++ b/5_TuningPrompting/output_data_v2.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+  <si>
+    <t>Tên Prompt</t>
+  </si>
   <si>
     <t>order</t>
   </si>
@@ -25,6 +28,12 @@
     <t>user_input</t>
   </si>
   <si>
+    <t>Example Given (from Backend )</t>
+  </si>
+  <si>
+    <t>Example Given (from ACA)</t>
+  </si>
+  <si>
     <t>system_prompt</t>
   </si>
   <si>
@@ -40,20 +49,78 @@
     <t>model_config</t>
   </si>
   <si>
-    <t>Robot: Bây giờ, thêm người ăn sáng cùng cậu nhé. Cậu nói: I eat breakfast with my family.
-user: "Eat breakfast only."</t>
-  </si>
-  <si>
-    <t>Bạn là 1 chuyên gia giảng dạy trẻ, nói chuyện với trẻ như 1 người bạn thân thiện, với mỗi trường hợp hội thoại tôi cần tạo câu fast response đệm, câu giờ trước khi trả về câu trả lời chính. 
-Giới hạn &lt;10 từ. Không tạo câu hỏi
-Xưng hô: cậu - tớ 
-Ví dụ: It's intersting, Oh i like apple too,....</t>
-  </si>
-  <si>
-    <t>That's cool, tớ cũng vậy đó</t>
-  </si>
-  <si>
-    <t>{"model": "llama-3.3-70b-versatile", "temperature": 0, "max_tokens": 2048, "top_p": 1, "frequency_penalty": 0.0, "presence_penalty": 0.0}</t>
+    <t>I went to the store yesterday to buy some groceries.</t>
+  </si>
+  <si>
+    <t>She is always smiling whenever I see her.</t>
+  </si>
+  <si>
+    <t>He don’t like to eat vegetables.</t>
+  </si>
+  <si>
+    <t>I didn’t knew about the meeting yesterday.</t>
+  </si>
+  <si>
+    <t>She enjoy playing the guitar on weekends.</t>
+  </si>
+  <si>
+    <t>They has been waiting for you since morning.</t>
+  </si>
+  <si>
+    <t>The cat sleep on the couch every night.</t>
+  </si>
+  <si>
+    <t>There is many reasons why I left the party.</t>
+  </si>
+  <si>
+    <t>She didn’t arrives on time for the meeting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Act as an English grammar teacher. Your task will be: 
+- Carefully analyze the given sentence. 
+- Check for grammar mistakes within the sentence. 
+- Context is not important. 
+INSTRUCTION 
+STEP 1: CHECK 
+- Check if the sentence is grammatically correct. 
+- Accept informal vocabulary usage as correct. 
+- Accept incorrect punctuation (. , ! ?...) as correct. 
+- If the sentence is grammatically correct, do not give any suggestion. 
+- If there is a grammar mistake, give the corrected version of the sentence. 
+STEP 2: RESPOND JSON TEMPLATE: 
+- Give a short, simple, brief explanation, and provide the corrected sentence if incorrect. 
++ If the sentence is correct, respond with: 
+{'explanation':null,'fixed_sentence':null,'correct_grammar':'true'} 
++ If the sentence is incorrect, never let fixed_sentence:null and respond with: 
+{'explanation':&lt;talk in Vietnamese, explain in detail why the given sentence is wrong and provide a corrected version&gt;,'fixed_sentence':&lt;must give example of a correct sentence, not null&gt;,'correct_grammar':'false'} 
+</t>
+  </si>
+  <si>
+    <t>{'explanation':null,'fixed_sentence':null,'correct_grammar':'true'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì \"don’t\" không phù hợp với chủ ngữ \"He\". Đối với chủ ngữ số ít như \"He\", chúng ta phải sử dụng \"doesn’t\". Do đó, câu đúng sẽ là \"He doesn’t like to eat vegetables.\"','fixed_sentence':'He doesn’t like to eat vegetables.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì động từ \"knew\" không nên được chia ở thì quá khứ hoàn thành với \"did\". Khi sử dụng \"did\" trong câu phủ định, động từ chính phải ở dạng nguyên thể. Do đó, câu đúng là \"I didn’t know about the meeting yesterday.\"','fixed_sentence':'I didn’t know about the meeting yesterday.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì động từ \"enjoy\" cần phải được chia theo chủ ngữ số ít \"She\". Đúng ra phải là \"enjoys\".','fixed_sentence':'She enjoys playing the guitar on weekends.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì chủ ngữ \"They\" là số nhiều, nên động từ \"has\" phải được thay bằng \"have\". Đúng là \"They have been waiting for you since morning.\"','fixed_sentence':'They have been waiting for you since morning.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì động từ \"sleep\" không được chia theo chủ ngữ \"The cat\". Đối với ngôi thứ ba số ít, động từ cần phải thêm \"s\" hoặc \"es\". Câu đúng là \"The cat sleeps on the couch every night.\"','fixed_sentence':'The cat sleeps on the couch every night.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì \"many\" không phù hợp với danh từ \"reasons\" trong ngữ cảnh này. Câu đúng nên sử dụng \"are\" thay vì \"is\" để phù hợp với số nhiều của danh từ. Câu sửa lại sẽ là: \"There are many reasons why I left the party.\"','fixed_sentence':'There are many reasons why I left the party.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{'explanation':'Câu này sai vì động từ \"arrives\" không phù hợp với thì quá khứ. Đúng ra phải dùng \"arrive\" để phù hợp với trợ động từ \"did\".','fixed_sentence':'She didn’t arrive on time for the meeting.','correct_grammar':'false'}</t>
+  </si>
+  <si>
+    <t>{"model": "gpt-4o-mini", "temperature": 0, "max_tokens": 2048, "top_p": 1, "frequency_penalty": 0.0, "presence_penalty": 0.0}</t>
   </si>
 </sst>
 </file>
@@ -411,13 +478,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,25 +509,224 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>2.301230669021606</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>0.8773629665374756</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>2.167365312576294</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>2.211078643798828</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>1.561907052993774</v>
+      </c>
+      <c r="L6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>2.272064447402954</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8">
+        <v>8.274530649185181</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9">
+        <v>2.844399452209473</v>
+      </c>
+      <c r="L9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0.5133044719696045</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>2.000658750534058</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>